<commit_message>
r type instructions finished
</commit_message>
<xml_diff>
--- a/Final-Project/instruction_set.xlsx
+++ b/Final-Project/instruction_set.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhodson/GitHub/digital-design/Final-Project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24214E34-06DB-384C-AE68-029E0FE03F8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="14730" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="171">
   <si>
     <t>Category</t>
   </si>
@@ -518,12 +524,21 @@
   </si>
   <si>
     <t>Multiplies (unsigned) $s by $t and stores the lower half of the result in $LO and the upper half in $HI.</t>
+  </si>
+  <si>
+    <t>31 downto 26</t>
+  </si>
+  <si>
+    <t>5 downto 0</t>
+  </si>
+  <si>
+    <t>r type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -545,7 +560,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +571,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -571,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -592,6 +613,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,6 +628,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -649,7 +679,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -682,9 +712,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,6 +764,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -892,28 +956,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1015"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="110" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="1" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.5" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="7" max="8" width="6.7109375" customWidth="1"/>
-    <col min="9" max="9" width="75.42578125" customWidth="1"/>
+    <col min="7" max="8" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="75.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="1"/>
+    <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,34 +1012,38 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="13"/>
+      <c r="L3" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>85</v>
       </c>
@@ -991,31 +1064,32 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="10"/>
+      <c r="I5" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1036,83 +1110,86 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="10"/>
+      <c r="I7" s="12" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="10"/>
+      <c r="I8" s="12" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
@@ -1136,31 +1213,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1184,31 +1262,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1232,103 +1311,107 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="10"/>
+      <c r="I15" s="12" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="10"/>
+      <c r="I16" s="12" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="39" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="10"/>
+      <c r="I18" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>158</v>
       </c>
@@ -1349,7 +1432,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="99" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>90</v>
       </c>
@@ -1370,79 +1453,82 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="39" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B21" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="10"/>
+      <c r="I21" s="12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="39" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="6" t="s">
+      <c r="H22" s="10"/>
+      <c r="I22" s="12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="39" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="6" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1453,7 +1539,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
@@ -1481,7 +1567,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>94</v>
       </c>
@@ -1505,10 +1591,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>118</v>
       </c>
@@ -1533,7 +1619,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>123</v>
       </c>
@@ -1554,7 +1640,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>127</v>
       </c>
@@ -1575,7 +1661,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>131</v>
       </c>
@@ -1596,7 +1682,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>135</v>
       </c>
@@ -1617,7 +1703,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
@@ -1640,11 +1726,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D34" s="8"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>142</v>
       </c>
@@ -1653,7 +1739,7 @@
       <c r="D35" s="8"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1674,7 +1760,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1695,2959 +1781,2960 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
+    <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="B38" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="6" t="s">
+      <c r="H38" s="10"/>
+      <c r="I38" s="12" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I79" s="6"/>
     </row>
-    <row r="80" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I88" s="6"/>
     </row>
-    <row r="89" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I89" s="6"/>
     </row>
-    <row r="90" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I91" s="6"/>
     </row>
-    <row r="92" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I93" s="6"/>
     </row>
-    <row r="94" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I94" s="6"/>
     </row>
-    <row r="95" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I95" s="6"/>
     </row>
-    <row r="96" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I96" s="6"/>
     </row>
-    <row r="97" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I97" s="6"/>
     </row>
-    <row r="98" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I100" s="6"/>
     </row>
-    <row r="101" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I101" s="6"/>
     </row>
-    <row r="102" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I102" s="6"/>
     </row>
-    <row r="103" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I103" s="6"/>
     </row>
-    <row r="104" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I104" s="6"/>
     </row>
-    <row r="105" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I105" s="6"/>
     </row>
-    <row r="106" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I106" s="6"/>
     </row>
-    <row r="107" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I107" s="6"/>
     </row>
-    <row r="108" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I108" s="6"/>
     </row>
-    <row r="109" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I109" s="6"/>
     </row>
-    <row r="110" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I110" s="6"/>
     </row>
-    <row r="111" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I111" s="6"/>
     </row>
-    <row r="112" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I115" s="6"/>
     </row>
-    <row r="116" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I116" s="6"/>
     </row>
-    <row r="117" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I117" s="6"/>
     </row>
-    <row r="118" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I118" s="6"/>
     </row>
-    <row r="119" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I119" s="6"/>
     </row>
-    <row r="120" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I120" s="6"/>
     </row>
-    <row r="121" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I121" s="6"/>
     </row>
-    <row r="122" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I122" s="6"/>
     </row>
-    <row r="123" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I123" s="6"/>
     </row>
-    <row r="124" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I124" s="6"/>
     </row>
-    <row r="125" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I125" s="6"/>
     </row>
-    <row r="126" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I126" s="6"/>
     </row>
-    <row r="127" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I127" s="6"/>
     </row>
-    <row r="128" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I128" s="6"/>
     </row>
-    <row r="129" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I129" s="6"/>
     </row>
-    <row r="130" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I130" s="6"/>
     </row>
-    <row r="131" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I131" s="6"/>
     </row>
-    <row r="132" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I132" s="6"/>
     </row>
-    <row r="133" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I133" s="6"/>
     </row>
-    <row r="134" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I134" s="6"/>
     </row>
-    <row r="135" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I135" s="6"/>
     </row>
-    <row r="136" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I136" s="6"/>
     </row>
-    <row r="137" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I137" s="6"/>
     </row>
-    <row r="138" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I138" s="6"/>
     </row>
-    <row r="139" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I139" s="6"/>
     </row>
-    <row r="140" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I140" s="6"/>
     </row>
-    <row r="141" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I141" s="6"/>
     </row>
-    <row r="142" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I142" s="6"/>
     </row>
-    <row r="143" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I143" s="6"/>
     </row>
-    <row r="144" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I144" s="6"/>
     </row>
-    <row r="145" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I145" s="6"/>
     </row>
-    <row r="146" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I146" s="6"/>
     </row>
-    <row r="147" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I147" s="6"/>
     </row>
-    <row r="148" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I148" s="6"/>
     </row>
-    <row r="149" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I149" s="6"/>
     </row>
-    <row r="150" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I150" s="6"/>
     </row>
-    <row r="151" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I151" s="6"/>
     </row>
-    <row r="152" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I152" s="6"/>
     </row>
-    <row r="153" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I153" s="6"/>
     </row>
-    <row r="154" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I154" s="6"/>
     </row>
-    <row r="155" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I155" s="6"/>
     </row>
-    <row r="156" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I156" s="6"/>
     </row>
-    <row r="157" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I157" s="6"/>
     </row>
-    <row r="158" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I158" s="6"/>
     </row>
-    <row r="159" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I159" s="6"/>
     </row>
-    <row r="160" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I160" s="6"/>
     </row>
-    <row r="161" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I161" s="6"/>
     </row>
-    <row r="162" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I162" s="6"/>
     </row>
-    <row r="163" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I163" s="6"/>
     </row>
-    <row r="164" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I164" s="6"/>
     </row>
-    <row r="165" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I165" s="2"/>
     </row>
-    <row r="166" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I166" s="2"/>
     </row>
-    <row r="167" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I167" s="2"/>
     </row>
-    <row r="168" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I168" s="2"/>
     </row>
-    <row r="169" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I169" s="2"/>
     </row>
-    <row r="170" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I170" s="2"/>
     </row>
-    <row r="171" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I171" s="2"/>
     </row>
-    <row r="172" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I172" s="2"/>
     </row>
-    <row r="173" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I173" s="2"/>
     </row>
-    <row r="174" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I174" s="2"/>
     </row>
-    <row r="175" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I175" s="2"/>
     </row>
-    <row r="176" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I176" s="2"/>
     </row>
-    <row r="177" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I177" s="2"/>
     </row>
-    <row r="178" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I178" s="2"/>
     </row>
-    <row r="179" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I179" s="2"/>
     </row>
-    <row r="180" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I180" s="2"/>
     </row>
-    <row r="181" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I181" s="2"/>
     </row>
-    <row r="182" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I182" s="2"/>
     </row>
-    <row r="183" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I183" s="2"/>
     </row>
-    <row r="184" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I184" s="2"/>
     </row>
-    <row r="185" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I185" s="2"/>
     </row>
-    <row r="186" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I186" s="2"/>
     </row>
-    <row r="187" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I187" s="2"/>
     </row>
-    <row r="188" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I188" s="2"/>
     </row>
-    <row r="189" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I189" s="2"/>
     </row>
-    <row r="190" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I190" s="2"/>
     </row>
-    <row r="191" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I191" s="2"/>
     </row>
-    <row r="192" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I192" s="2"/>
     </row>
-    <row r="193" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I193" s="2"/>
     </row>
-    <row r="194" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I194" s="2"/>
     </row>
-    <row r="195" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I195" s="2"/>
     </row>
-    <row r="196" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I196" s="2"/>
     </row>
-    <row r="197" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I197" s="2"/>
     </row>
-    <row r="198" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I198" s="2"/>
     </row>
-    <row r="199" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I199" s="2"/>
     </row>
-    <row r="200" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I200" s="2"/>
     </row>
-    <row r="201" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I201" s="2"/>
     </row>
-    <row r="202" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I202" s="2"/>
     </row>
-    <row r="203" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I203" s="2"/>
     </row>
-    <row r="204" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I204" s="2"/>
     </row>
-    <row r="205" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I205" s="2"/>
     </row>
-    <row r="206" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I206" s="2"/>
     </row>
-    <row r="207" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I207" s="2"/>
     </row>
-    <row r="208" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I208" s="2"/>
     </row>
-    <row r="209" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I209" s="2"/>
     </row>
-    <row r="210" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I210" s="2"/>
     </row>
-    <row r="211" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I211" s="2"/>
     </row>
-    <row r="212" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I212" s="2"/>
     </row>
-    <row r="213" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I213" s="2"/>
     </row>
-    <row r="214" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I214" s="2"/>
     </row>
-    <row r="215" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I215" s="2"/>
     </row>
-    <row r="216" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I216" s="2"/>
     </row>
-    <row r="217" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I217" s="2"/>
     </row>
-    <row r="218" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I218" s="2"/>
     </row>
-    <row r="219" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I219" s="2"/>
     </row>
-    <row r="220" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I220" s="2"/>
     </row>
-    <row r="221" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I221" s="2"/>
     </row>
-    <row r="222" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I222" s="2"/>
     </row>
-    <row r="223" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I223" s="2"/>
     </row>
-    <row r="224" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I224" s="2"/>
     </row>
-    <row r="225" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I225" s="2"/>
     </row>
-    <row r="226" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I226" s="2"/>
     </row>
-    <row r="227" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I227" s="2"/>
     </row>
-    <row r="228" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I228" s="2"/>
     </row>
-    <row r="229" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I229" s="2"/>
     </row>
-    <row r="230" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I230" s="2"/>
     </row>
-    <row r="231" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I231" s="2"/>
     </row>
-    <row r="232" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I232" s="2"/>
     </row>
-    <row r="233" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I233" s="2"/>
     </row>
-    <row r="234" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I234" s="2"/>
     </row>
-    <row r="235" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I235" s="2"/>
     </row>
-    <row r="236" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I236" s="2"/>
     </row>
-    <row r="237" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I237" s="2"/>
     </row>
-    <row r="238" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I238" s="2"/>
     </row>
-    <row r="239" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I239" s="2"/>
     </row>
-    <row r="240" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I240" s="2"/>
     </row>
-    <row r="241" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I241" s="2"/>
     </row>
-    <row r="242" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I242" s="2"/>
     </row>
-    <row r="243" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I243" s="2"/>
     </row>
-    <row r="244" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I244" s="2"/>
     </row>
-    <row r="245" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I245" s="2"/>
     </row>
-    <row r="246" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I246" s="2"/>
     </row>
-    <row r="247" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I247" s="2"/>
     </row>
-    <row r="248" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I248" s="2"/>
     </row>
-    <row r="249" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I249" s="2"/>
     </row>
-    <row r="250" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I250" s="2"/>
     </row>
-    <row r="251" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I251" s="2"/>
     </row>
-    <row r="252" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I252" s="2"/>
     </row>
-    <row r="253" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I253" s="2"/>
     </row>
-    <row r="254" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I254" s="2"/>
     </row>
-    <row r="255" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I255" s="2"/>
     </row>
-    <row r="256" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I256" s="2"/>
     </row>
-    <row r="257" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I257" s="2"/>
     </row>
-    <row r="258" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I258" s="2"/>
     </row>
-    <row r="259" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I259" s="2"/>
     </row>
-    <row r="260" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I260" s="2"/>
     </row>
-    <row r="261" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I261" s="2"/>
     </row>
-    <row r="262" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I262" s="2"/>
     </row>
-    <row r="263" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I263" s="2"/>
     </row>
-    <row r="264" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I264" s="2"/>
     </row>
-    <row r="265" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I265" s="2"/>
     </row>
-    <row r="266" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I266" s="2"/>
     </row>
-    <row r="267" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I267" s="2"/>
     </row>
-    <row r="268" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I268" s="2"/>
     </row>
-    <row r="269" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I269" s="2"/>
     </row>
-    <row r="270" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I270" s="2"/>
     </row>
-    <row r="271" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I271" s="2"/>
     </row>
-    <row r="272" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I272" s="2"/>
     </row>
-    <row r="273" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I273" s="2"/>
     </row>
-    <row r="274" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I274" s="2"/>
     </row>
-    <row r="275" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I275" s="2"/>
     </row>
-    <row r="276" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I276" s="2"/>
     </row>
-    <row r="277" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I277" s="2"/>
     </row>
-    <row r="278" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I278" s="2"/>
     </row>
-    <row r="279" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I279" s="2"/>
     </row>
-    <row r="280" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I280" s="2"/>
     </row>
-    <row r="281" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I281" s="2"/>
     </row>
-    <row r="282" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I282" s="2"/>
     </row>
-    <row r="283" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I283" s="2"/>
     </row>
-    <row r="284" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I284" s="2"/>
     </row>
-    <row r="285" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I285" s="2"/>
     </row>
-    <row r="286" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I286" s="2"/>
     </row>
-    <row r="287" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I287" s="2"/>
     </row>
-    <row r="288" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I288" s="2"/>
     </row>
-    <row r="289" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I289" s="2"/>
     </row>
-    <row r="290" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I290" s="2"/>
     </row>
-    <row r="291" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I291" s="2"/>
     </row>
-    <row r="292" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I292" s="2"/>
     </row>
-    <row r="293" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I293" s="2"/>
     </row>
-    <row r="294" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="294" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I294" s="2"/>
     </row>
-    <row r="295" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I295" s="2"/>
     </row>
-    <row r="296" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="296" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I296" s="2"/>
     </row>
-    <row r="297" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="297" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I297" s="2"/>
     </row>
-    <row r="298" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I298" s="2"/>
     </row>
-    <row r="299" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I299" s="2"/>
     </row>
-    <row r="300" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I300" s="2"/>
     </row>
-    <row r="301" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I301" s="2"/>
     </row>
-    <row r="302" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I302" s="2"/>
     </row>
-    <row r="303" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="303" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I303" s="2"/>
     </row>
-    <row r="304" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="304" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I304" s="2"/>
     </row>
-    <row r="305" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="305" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I305" s="2"/>
     </row>
-    <row r="306" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="306" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I306" s="2"/>
     </row>
-    <row r="307" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="307" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I307" s="2"/>
     </row>
-    <row r="308" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="308" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I308" s="2"/>
     </row>
-    <row r="309" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="309" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I309" s="2"/>
     </row>
-    <row r="310" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="310" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I310" s="2"/>
     </row>
-    <row r="311" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="311" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I311" s="2"/>
     </row>
-    <row r="312" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="312" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I312" s="2"/>
     </row>
-    <row r="313" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="313" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I313" s="2"/>
     </row>
-    <row r="314" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="314" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I314" s="2"/>
     </row>
-    <row r="315" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="315" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I315" s="2"/>
     </row>
-    <row r="316" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="316" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I316" s="2"/>
     </row>
-    <row r="317" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="317" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I317" s="2"/>
     </row>
-    <row r="318" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="318" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I318" s="2"/>
     </row>
-    <row r="319" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="319" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I319" s="2"/>
     </row>
-    <row r="320" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="320" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I320" s="2"/>
     </row>
-    <row r="321" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="321" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I321" s="2"/>
     </row>
-    <row r="322" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="322" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I322" s="2"/>
     </row>
-    <row r="323" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="323" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I323" s="2"/>
     </row>
-    <row r="324" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="324" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I324" s="2"/>
     </row>
-    <row r="325" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="325" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I325" s="2"/>
     </row>
-    <row r="326" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="326" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I326" s="2"/>
     </row>
-    <row r="327" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="327" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I327" s="2"/>
     </row>
-    <row r="328" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="328" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I328" s="2"/>
     </row>
-    <row r="329" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="329" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I329" s="2"/>
     </row>
-    <row r="330" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="330" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I330" s="2"/>
     </row>
-    <row r="331" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="331" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I331" s="2"/>
     </row>
-    <row r="332" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="332" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I332" s="2"/>
     </row>
-    <row r="333" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="333" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I333" s="2"/>
     </row>
-    <row r="334" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="334" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I334" s="2"/>
     </row>
-    <row r="335" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="335" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I335" s="2"/>
     </row>
-    <row r="336" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="336" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I336" s="2"/>
     </row>
-    <row r="337" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="337" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I337" s="2"/>
     </row>
-    <row r="338" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="338" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I338" s="2"/>
     </row>
-    <row r="339" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="339" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I339" s="2"/>
     </row>
-    <row r="340" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="340" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I340" s="2"/>
     </row>
-    <row r="341" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="341" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I341" s="2"/>
     </row>
-    <row r="342" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="342" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I342" s="2"/>
     </row>
-    <row r="343" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="343" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I343" s="2"/>
     </row>
-    <row r="344" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="344" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I344" s="2"/>
     </row>
-    <row r="345" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="345" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I345" s="2"/>
     </row>
-    <row r="346" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="346" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I346" s="2"/>
     </row>
-    <row r="347" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="347" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I347" s="2"/>
     </row>
-    <row r="348" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="348" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I348" s="2"/>
     </row>
-    <row r="349" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="349" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I349" s="2"/>
     </row>
-    <row r="350" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="350" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I350" s="2"/>
     </row>
-    <row r="351" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="351" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I351" s="2"/>
     </row>
-    <row r="352" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="352" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I352" s="2"/>
     </row>
-    <row r="353" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="353" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I353" s="2"/>
     </row>
-    <row r="354" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="354" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I354" s="2"/>
     </row>
-    <row r="355" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="355" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I355" s="2"/>
     </row>
-    <row r="356" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="356" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I356" s="2"/>
     </row>
-    <row r="357" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="357" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I357" s="2"/>
     </row>
-    <row r="358" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="358" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I358" s="2"/>
     </row>
-    <row r="359" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="359" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I359" s="2"/>
     </row>
-    <row r="360" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="360" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I360" s="2"/>
     </row>
-    <row r="361" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="361" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I361" s="2"/>
     </row>
-    <row r="362" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="362" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I362" s="2"/>
     </row>
-    <row r="363" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="363" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I363" s="2"/>
     </row>
-    <row r="364" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="364" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I364" s="2"/>
     </row>
-    <row r="365" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="365" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I365" s="2"/>
     </row>
-    <row r="366" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="366" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I366" s="2"/>
     </row>
-    <row r="367" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="367" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I367" s="2"/>
     </row>
-    <row r="368" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="368" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I368" s="2"/>
     </row>
-    <row r="369" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="369" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I369" s="2"/>
     </row>
-    <row r="370" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="370" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I370" s="2"/>
     </row>
-    <row r="371" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="371" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I371" s="2"/>
     </row>
-    <row r="372" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="372" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I372" s="2"/>
     </row>
-    <row r="373" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="373" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I373" s="2"/>
     </row>
-    <row r="374" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="374" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I374" s="2"/>
     </row>
-    <row r="375" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="375" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I375" s="2"/>
     </row>
-    <row r="376" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="376" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I376" s="2"/>
     </row>
-    <row r="377" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="377" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I377" s="2"/>
     </row>
-    <row r="378" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="378" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I378" s="2"/>
     </row>
-    <row r="379" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="379" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I379" s="2"/>
     </row>
-    <row r="380" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="380" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I380" s="2"/>
     </row>
-    <row r="381" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="381" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I381" s="2"/>
     </row>
-    <row r="382" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="382" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I382" s="2"/>
     </row>
-    <row r="383" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="383" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I383" s="2"/>
     </row>
-    <row r="384" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="384" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I384" s="2"/>
     </row>
-    <row r="385" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="385" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I385" s="2"/>
     </row>
-    <row r="386" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I386" s="2"/>
     </row>
-    <row r="387" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="387" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I387" s="2"/>
     </row>
-    <row r="388" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="388" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I388" s="2"/>
     </row>
-    <row r="389" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="389" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I389" s="2"/>
     </row>
-    <row r="390" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="390" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I390" s="2"/>
     </row>
-    <row r="391" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="391" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I391" s="2"/>
     </row>
-    <row r="392" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="392" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I392" s="2"/>
     </row>
-    <row r="393" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="393" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I393" s="2"/>
     </row>
-    <row r="394" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="394" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I394" s="2"/>
     </row>
-    <row r="395" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="395" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I395" s="2"/>
     </row>
-    <row r="396" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="396" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I396" s="2"/>
     </row>
-    <row r="397" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="397" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I397" s="2"/>
     </row>
-    <row r="398" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="398" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I398" s="2"/>
     </row>
-    <row r="399" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="399" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I399" s="2"/>
     </row>
-    <row r="400" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="400" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I400" s="2"/>
     </row>
-    <row r="401" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="401" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I401" s="2"/>
     </row>
-    <row r="402" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="402" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I402" s="2"/>
     </row>
-    <row r="403" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="403" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I403" s="2"/>
     </row>
-    <row r="404" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="404" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I404" s="2"/>
     </row>
-    <row r="405" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="405" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I405" s="2"/>
     </row>
-    <row r="406" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="406" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I406" s="2"/>
     </row>
-    <row r="407" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="407" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I407" s="2"/>
     </row>
-    <row r="408" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="408" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I408" s="2"/>
     </row>
-    <row r="409" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="409" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I409" s="2"/>
     </row>
-    <row r="410" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="410" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I410" s="2"/>
     </row>
-    <row r="411" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="411" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I411" s="2"/>
     </row>
-    <row r="412" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="412" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I412" s="2"/>
     </row>
-    <row r="413" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="413" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I413" s="2"/>
     </row>
-    <row r="414" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="414" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I414" s="2"/>
     </row>
-    <row r="415" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="415" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I415" s="2"/>
     </row>
-    <row r="416" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="416" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I416" s="2"/>
     </row>
-    <row r="417" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="417" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I417" s="2"/>
     </row>
-    <row r="418" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="418" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I418" s="2"/>
     </row>
-    <row r="419" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="419" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I419" s="2"/>
     </row>
-    <row r="420" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="420" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I420" s="2"/>
     </row>
-    <row r="421" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="421" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I421" s="2"/>
     </row>
-    <row r="422" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="422" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I422" s="2"/>
     </row>
-    <row r="423" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="423" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I423" s="2"/>
     </row>
-    <row r="424" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="424" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I424" s="2"/>
     </row>
-    <row r="425" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="425" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I425" s="2"/>
     </row>
-    <row r="426" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="426" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I426" s="2"/>
     </row>
-    <row r="427" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="427" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I427" s="2"/>
     </row>
-    <row r="428" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="428" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I428" s="2"/>
     </row>
-    <row r="429" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="429" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I429" s="2"/>
     </row>
-    <row r="430" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="430" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I430" s="2"/>
     </row>
-    <row r="431" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="431" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I431" s="2"/>
     </row>
-    <row r="432" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="432" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I432" s="2"/>
     </row>
-    <row r="433" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="433" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I433" s="2"/>
     </row>
-    <row r="434" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="434" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I434" s="2"/>
     </row>
-    <row r="435" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="435" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I435" s="2"/>
     </row>
-    <row r="436" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="436" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I436" s="2"/>
     </row>
-    <row r="437" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="437" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I437" s="2"/>
     </row>
-    <row r="438" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="438" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I438" s="2"/>
     </row>
-    <row r="439" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="439" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I439" s="2"/>
     </row>
-    <row r="440" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="440" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I440" s="2"/>
     </row>
-    <row r="441" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="441" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I441" s="2"/>
     </row>
-    <row r="442" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="442" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I442" s="2"/>
     </row>
-    <row r="443" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="443" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I443" s="2"/>
     </row>
-    <row r="444" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="444" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I444" s="2"/>
     </row>
-    <row r="445" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="445" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I445" s="2"/>
     </row>
-    <row r="446" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="446" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I446" s="2"/>
     </row>
-    <row r="447" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="447" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I447" s="2"/>
     </row>
-    <row r="448" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="448" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I448" s="2"/>
     </row>
-    <row r="449" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="449" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I449" s="2"/>
     </row>
-    <row r="450" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="450" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I450" s="2"/>
     </row>
-    <row r="451" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="451" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I451" s="2"/>
     </row>
-    <row r="452" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="452" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I452" s="2"/>
     </row>
-    <row r="453" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="453" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I453" s="2"/>
     </row>
-    <row r="454" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="454" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I454" s="2"/>
     </row>
-    <row r="455" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="455" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I455" s="2"/>
     </row>
-    <row r="456" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="456" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I456" s="2"/>
     </row>
-    <row r="457" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="457" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I457" s="2"/>
     </row>
-    <row r="458" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="458" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I458" s="2"/>
     </row>
-    <row r="459" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="459" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I459" s="2"/>
     </row>
-    <row r="460" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="460" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I460" s="2"/>
     </row>
-    <row r="461" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="461" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I461" s="2"/>
     </row>
-    <row r="462" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="462" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I462" s="2"/>
     </row>
-    <row r="463" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="463" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I463" s="2"/>
     </row>
-    <row r="464" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="464" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I464" s="2"/>
     </row>
-    <row r="465" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="465" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I465" s="2"/>
     </row>
-    <row r="466" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="466" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I466" s="2"/>
     </row>
-    <row r="467" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="467" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I467" s="2"/>
     </row>
-    <row r="468" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="468" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I468" s="2"/>
     </row>
-    <row r="469" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="469" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I469" s="2"/>
     </row>
-    <row r="470" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="470" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I470" s="2"/>
     </row>
-    <row r="471" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="471" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I471" s="2"/>
     </row>
-    <row r="472" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="472" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I472" s="2"/>
     </row>
-    <row r="473" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="473" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I473" s="2"/>
     </row>
-    <row r="474" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="474" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I474" s="2"/>
     </row>
-    <row r="475" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="475" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I475" s="2"/>
     </row>
-    <row r="476" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="476" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I476" s="2"/>
     </row>
-    <row r="477" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="477" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I477" s="2"/>
     </row>
-    <row r="478" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="478" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I478" s="2"/>
     </row>
-    <row r="479" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="479" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I479" s="2"/>
     </row>
-    <row r="480" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="480" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I480" s="2"/>
     </row>
-    <row r="481" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="481" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I481" s="2"/>
     </row>
-    <row r="482" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="482" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I482" s="2"/>
     </row>
-    <row r="483" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="483" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I483" s="2"/>
     </row>
-    <row r="484" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="484" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I484" s="2"/>
     </row>
-    <row r="485" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="485" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I485" s="2"/>
     </row>
-    <row r="486" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="486" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I486" s="2"/>
     </row>
-    <row r="487" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="487" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I487" s="2"/>
     </row>
-    <row r="488" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="488" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I488" s="2"/>
     </row>
-    <row r="489" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="489" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I489" s="2"/>
     </row>
-    <row r="490" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="490" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I490" s="2"/>
     </row>
-    <row r="491" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="491" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I491" s="2"/>
     </row>
-    <row r="492" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="492" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I492" s="2"/>
     </row>
-    <row r="493" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="493" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I493" s="2"/>
     </row>
-    <row r="494" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="494" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I494" s="2"/>
     </row>
-    <row r="495" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="495" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I495" s="2"/>
     </row>
-    <row r="496" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="496" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I496" s="2"/>
     </row>
-    <row r="497" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="497" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I497" s="2"/>
     </row>
-    <row r="498" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="498" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I498" s="2"/>
     </row>
-    <row r="499" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="499" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I499" s="2"/>
     </row>
-    <row r="500" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="500" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I500" s="2"/>
     </row>
-    <row r="501" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="501" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I501" s="2"/>
     </row>
-    <row r="502" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="502" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I502" s="2"/>
     </row>
-    <row r="503" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="503" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I503" s="2"/>
     </row>
-    <row r="504" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="504" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I504" s="2"/>
     </row>
-    <row r="505" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="505" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I505" s="2"/>
     </row>
-    <row r="506" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="506" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I506" s="2"/>
     </row>
-    <row r="507" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="507" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I507" s="2"/>
     </row>
-    <row r="508" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="508" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I508" s="2"/>
     </row>
-    <row r="509" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="509" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I509" s="2"/>
     </row>
-    <row r="510" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="510" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I510" s="2"/>
     </row>
-    <row r="511" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="511" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I511" s="2"/>
     </row>
-    <row r="512" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="512" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I512" s="2"/>
     </row>
-    <row r="513" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="513" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I513" s="2"/>
     </row>
-    <row r="514" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="514" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I514" s="2"/>
     </row>
-    <row r="515" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="515" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I515" s="2"/>
     </row>
-    <row r="516" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="516" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I516" s="2"/>
     </row>
-    <row r="517" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="517" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I517" s="2"/>
     </row>
-    <row r="518" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="518" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I518" s="2"/>
     </row>
-    <row r="519" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="519" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I519" s="2"/>
     </row>
-    <row r="520" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="520" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I520" s="2"/>
     </row>
-    <row r="521" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="521" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I521" s="2"/>
     </row>
-    <row r="522" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="522" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I522" s="2"/>
     </row>
-    <row r="523" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="523" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I523" s="2"/>
     </row>
-    <row r="524" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="524" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I524" s="2"/>
     </row>
-    <row r="525" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="525" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I525" s="2"/>
     </row>
-    <row r="526" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="526" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I526" s="2"/>
     </row>
-    <row r="527" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="527" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I527" s="2"/>
     </row>
-    <row r="528" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="528" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I528" s="2"/>
     </row>
-    <row r="529" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="529" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I529" s="2"/>
     </row>
-    <row r="530" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="530" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I530" s="2"/>
     </row>
-    <row r="531" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="531" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I531" s="2"/>
     </row>
-    <row r="532" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="532" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I532" s="2"/>
     </row>
-    <row r="533" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="533" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I533" s="2"/>
     </row>
-    <row r="534" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="534" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I534" s="2"/>
     </row>
-    <row r="535" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="535" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I535" s="2"/>
     </row>
-    <row r="536" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="536" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I536" s="2"/>
     </row>
-    <row r="537" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="537" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I537" s="2"/>
     </row>
-    <row r="538" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="538" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I538" s="2"/>
     </row>
-    <row r="539" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="539" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I539" s="2"/>
     </row>
-    <row r="540" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="540" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I540" s="2"/>
     </row>
-    <row r="541" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="541" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I541" s="2"/>
     </row>
-    <row r="542" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="542" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I542" s="2"/>
     </row>
-    <row r="543" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="543" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I543" s="2"/>
     </row>
-    <row r="544" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="544" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I544" s="2"/>
     </row>
-    <row r="545" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="545" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I545" s="2"/>
     </row>
-    <row r="546" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="546" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I546" s="2"/>
     </row>
-    <row r="547" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="547" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I547" s="2"/>
     </row>
-    <row r="548" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="548" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I548" s="2"/>
     </row>
-    <row r="549" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="549" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I549" s="2"/>
     </row>
-    <row r="550" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="550" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I550" s="2"/>
     </row>
-    <row r="551" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="551" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I551" s="2"/>
     </row>
-    <row r="552" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="552" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I552" s="2"/>
     </row>
-    <row r="553" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="553" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I553" s="2"/>
     </row>
-    <row r="554" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="554" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I554" s="2"/>
     </row>
-    <row r="555" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="555" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I555" s="2"/>
     </row>
-    <row r="556" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="556" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I556" s="2"/>
     </row>
-    <row r="557" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="557" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I557" s="2"/>
     </row>
-    <row r="558" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="558" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I558" s="2"/>
     </row>
-    <row r="559" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="559" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I559" s="2"/>
     </row>
-    <row r="560" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="560" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I560" s="2"/>
     </row>
-    <row r="561" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="561" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I561" s="2"/>
     </row>
-    <row r="562" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="562" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I562" s="2"/>
     </row>
-    <row r="563" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="563" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I563" s="2"/>
     </row>
-    <row r="564" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="564" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I564" s="2"/>
     </row>
-    <row r="565" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="565" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I565" s="2"/>
     </row>
-    <row r="566" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="566" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I566" s="2"/>
     </row>
-    <row r="567" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="567" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I567" s="2"/>
     </row>
-    <row r="568" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="568" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I568" s="2"/>
     </row>
-    <row r="569" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="569" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I569" s="2"/>
     </row>
-    <row r="570" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="570" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I570" s="2"/>
     </row>
-    <row r="571" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="571" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I571" s="2"/>
     </row>
-    <row r="572" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="572" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I572" s="2"/>
     </row>
-    <row r="573" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="573" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I573" s="2"/>
     </row>
-    <row r="574" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="574" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I574" s="2"/>
     </row>
-    <row r="575" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="575" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I575" s="2"/>
     </row>
-    <row r="576" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="576" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I576" s="2"/>
     </row>
-    <row r="577" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="577" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I577" s="2"/>
     </row>
-    <row r="578" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="578" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I578" s="2"/>
     </row>
-    <row r="579" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="579" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I579" s="2"/>
     </row>
-    <row r="580" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="580" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I580" s="2"/>
     </row>
-    <row r="581" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="581" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I581" s="2"/>
     </row>
-    <row r="582" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="582" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I582" s="2"/>
     </row>
-    <row r="583" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="583" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I583" s="2"/>
     </row>
-    <row r="584" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="584" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I584" s="2"/>
     </row>
-    <row r="585" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="585" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I585" s="2"/>
     </row>
-    <row r="586" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="586" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I586" s="2"/>
     </row>
-    <row r="587" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="587" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I587" s="2"/>
     </row>
-    <row r="588" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="588" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I588" s="2"/>
     </row>
-    <row r="589" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="589" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I589" s="2"/>
     </row>
-    <row r="590" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="590" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I590" s="2"/>
     </row>
-    <row r="591" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="591" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I591" s="2"/>
     </row>
-    <row r="592" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="592" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I592" s="2"/>
     </row>
-    <row r="593" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="593" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I593" s="2"/>
     </row>
-    <row r="594" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="594" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I594" s="2"/>
     </row>
-    <row r="595" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="595" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I595" s="2"/>
     </row>
-    <row r="596" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="596" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I596" s="2"/>
     </row>
-    <row r="597" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="597" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I597" s="2"/>
     </row>
-    <row r="598" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="598" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I598" s="2"/>
     </row>
-    <row r="599" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="599" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I599" s="2"/>
     </row>
-    <row r="600" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="600" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I600" s="2"/>
     </row>
-    <row r="601" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="601" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I601" s="2"/>
     </row>
-    <row r="602" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="602" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I602" s="2"/>
     </row>
-    <row r="603" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="603" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I603" s="2"/>
     </row>
-    <row r="604" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="604" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I604" s="2"/>
     </row>
-    <row r="605" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="605" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I605" s="2"/>
     </row>
-    <row r="606" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="606" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I606" s="2"/>
     </row>
-    <row r="607" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="607" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I607" s="2"/>
     </row>
-    <row r="608" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="608" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I608" s="2"/>
     </row>
-    <row r="609" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="609" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I609" s="2"/>
     </row>
-    <row r="610" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="610" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I610" s="2"/>
     </row>
-    <row r="611" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="611" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I611" s="2"/>
     </row>
-    <row r="612" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="612" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I612" s="2"/>
     </row>
-    <row r="613" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="613" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I613" s="2"/>
     </row>
-    <row r="614" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="614" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I614" s="2"/>
     </row>
-    <row r="615" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="615" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I615" s="2"/>
     </row>
-    <row r="616" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="616" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I616" s="2"/>
     </row>
-    <row r="617" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="617" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I617" s="2"/>
     </row>
-    <row r="618" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="618" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I618" s="2"/>
     </row>
-    <row r="619" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="619" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I619" s="2"/>
     </row>
-    <row r="620" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="620" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I620" s="2"/>
     </row>
-    <row r="621" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="621" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I621" s="2"/>
     </row>
-    <row r="622" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="622" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I622" s="2"/>
     </row>
-    <row r="623" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="623" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I623" s="2"/>
     </row>
-    <row r="624" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="624" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I624" s="2"/>
     </row>
-    <row r="625" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="625" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I625" s="2"/>
     </row>
-    <row r="626" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="626" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I626" s="2"/>
     </row>
-    <row r="627" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="627" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I627" s="2"/>
     </row>
-    <row r="628" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="628" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I628" s="2"/>
     </row>
-    <row r="629" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="629" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I629" s="2"/>
     </row>
-    <row r="630" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="630" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I630" s="2"/>
     </row>
-    <row r="631" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="631" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I631" s="2"/>
     </row>
-    <row r="632" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="632" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I632" s="2"/>
     </row>
-    <row r="633" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="633" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I633" s="2"/>
     </row>
-    <row r="634" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="634" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I634" s="2"/>
     </row>
-    <row r="635" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="635" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I635" s="2"/>
     </row>
-    <row r="636" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="636" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I636" s="2"/>
     </row>
-    <row r="637" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="637" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I637" s="2"/>
     </row>
-    <row r="638" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="638" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I638" s="2"/>
     </row>
-    <row r="639" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="639" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I639" s="2"/>
     </row>
-    <row r="640" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="640" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I640" s="2"/>
     </row>
-    <row r="641" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="641" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I641" s="2"/>
     </row>
-    <row r="642" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="642" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I642" s="2"/>
     </row>
-    <row r="643" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="643" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I643" s="2"/>
     </row>
-    <row r="644" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="644" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I644" s="2"/>
     </row>
-    <row r="645" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="645" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I645" s="2"/>
     </row>
-    <row r="646" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="646" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I646" s="2"/>
     </row>
-    <row r="647" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="647" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I647" s="2"/>
     </row>
-    <row r="648" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="648" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I648" s="2"/>
     </row>
-    <row r="649" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="649" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I649" s="2"/>
     </row>
-    <row r="650" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="650" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I650" s="2"/>
     </row>
-    <row r="651" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="651" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I651" s="2"/>
     </row>
-    <row r="652" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="652" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I652" s="2"/>
     </row>
-    <row r="653" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="653" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I653" s="2"/>
     </row>
-    <row r="654" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="654" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I654" s="2"/>
     </row>
-    <row r="655" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="655" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I655" s="2"/>
     </row>
-    <row r="656" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="656" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I656" s="2"/>
     </row>
-    <row r="657" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="657" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I657" s="2"/>
     </row>
-    <row r="658" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="658" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I658" s="2"/>
     </row>
-    <row r="659" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="659" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I659" s="2"/>
     </row>
-    <row r="660" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="660" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I660" s="2"/>
     </row>
-    <row r="661" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="661" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I661" s="2"/>
     </row>
-    <row r="662" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="662" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I662" s="2"/>
     </row>
-    <row r="663" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="663" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I663" s="2"/>
     </row>
-    <row r="664" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="664" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I664" s="2"/>
     </row>
-    <row r="665" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="665" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I665" s="2"/>
     </row>
-    <row r="666" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="666" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I666" s="2"/>
     </row>
-    <row r="667" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="667" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I667" s="2"/>
     </row>
-    <row r="668" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="668" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I668" s="2"/>
     </row>
-    <row r="669" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="669" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I669" s="2"/>
     </row>
-    <row r="670" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="670" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I670" s="2"/>
     </row>
-    <row r="671" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="671" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I671" s="2"/>
     </row>
-    <row r="672" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="672" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I672" s="2"/>
     </row>
-    <row r="673" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="673" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I673" s="2"/>
     </row>
-    <row r="674" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="674" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I674" s="2"/>
     </row>
-    <row r="675" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="675" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I675" s="2"/>
     </row>
-    <row r="676" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="676" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I676" s="2"/>
     </row>
-    <row r="677" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="677" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I677" s="2"/>
     </row>
-    <row r="678" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="678" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I678" s="2"/>
     </row>
-    <row r="679" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="679" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I679" s="2"/>
     </row>
-    <row r="680" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="680" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I680" s="2"/>
     </row>
-    <row r="681" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="681" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I681" s="2"/>
     </row>
-    <row r="682" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="682" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I682" s="2"/>
     </row>
-    <row r="683" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="683" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I683" s="2"/>
     </row>
-    <row r="684" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="684" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I684" s="2"/>
     </row>
-    <row r="685" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="685" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I685" s="2"/>
     </row>
-    <row r="686" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="686" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I686" s="2"/>
     </row>
-    <row r="687" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="687" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I687" s="2"/>
     </row>
-    <row r="688" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="688" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I688" s="2"/>
     </row>
-    <row r="689" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="689" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I689" s="2"/>
     </row>
-    <row r="690" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="690" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I690" s="2"/>
     </row>
-    <row r="691" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="691" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I691" s="2"/>
     </row>
-    <row r="692" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="692" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I692" s="2"/>
     </row>
-    <row r="693" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="693" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I693" s="2"/>
     </row>
-    <row r="694" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="694" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I694" s="2"/>
     </row>
-    <row r="695" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="695" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I695" s="2"/>
     </row>
-    <row r="696" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="696" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I696" s="2"/>
     </row>
-    <row r="697" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="697" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I697" s="2"/>
     </row>
-    <row r="698" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="698" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I698" s="2"/>
     </row>
-    <row r="699" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="699" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I699" s="2"/>
     </row>
-    <row r="700" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="700" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I700" s="2"/>
     </row>
-    <row r="701" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="701" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I701" s="2"/>
     </row>
-    <row r="702" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="702" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I702" s="2"/>
     </row>
-    <row r="703" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="703" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I703" s="2"/>
     </row>
-    <row r="704" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="704" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I704" s="2"/>
     </row>
-    <row r="705" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="705" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I705" s="2"/>
     </row>
-    <row r="706" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="706" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I706" s="2"/>
     </row>
-    <row r="707" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="707" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I707" s="2"/>
     </row>
-    <row r="708" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="708" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I708" s="2"/>
     </row>
-    <row r="709" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="709" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I709" s="2"/>
     </row>
-    <row r="710" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="710" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I710" s="2"/>
     </row>
-    <row r="711" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="711" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I711" s="2"/>
     </row>
-    <row r="712" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="712" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I712" s="2"/>
     </row>
-    <row r="713" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="713" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I713" s="2"/>
     </row>
-    <row r="714" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="714" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I714" s="2"/>
     </row>
-    <row r="715" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="715" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I715" s="2"/>
     </row>
-    <row r="716" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="716" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I716" s="2"/>
     </row>
-    <row r="717" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="717" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I717" s="2"/>
     </row>
-    <row r="718" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="718" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I718" s="2"/>
     </row>
-    <row r="719" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="719" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I719" s="2"/>
     </row>
-    <row r="720" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="720" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I720" s="2"/>
     </row>
-    <row r="721" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="721" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I721" s="2"/>
     </row>
-    <row r="722" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="722" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I722" s="2"/>
     </row>
-    <row r="723" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="723" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I723" s="2"/>
     </row>
-    <row r="724" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="724" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I724" s="2"/>
     </row>
-    <row r="725" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="725" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I725" s="2"/>
     </row>
-    <row r="726" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="726" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I726" s="2"/>
     </row>
-    <row r="727" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="727" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I727" s="2"/>
     </row>
-    <row r="728" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="728" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I728" s="2"/>
     </row>
-    <row r="729" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="729" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I729" s="2"/>
     </row>
-    <row r="730" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="730" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I730" s="2"/>
     </row>
-    <row r="731" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="731" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I731" s="2"/>
     </row>
-    <row r="732" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="732" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I732" s="2"/>
     </row>
-    <row r="733" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="733" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I733" s="2"/>
     </row>
-    <row r="734" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="734" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I734" s="2"/>
     </row>
-    <row r="735" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="735" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I735" s="2"/>
     </row>
-    <row r="736" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="736" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I736" s="2"/>
     </row>
-    <row r="737" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="737" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I737" s="2"/>
     </row>
-    <row r="738" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="738" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I738" s="2"/>
     </row>
-    <row r="739" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="739" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I739" s="2"/>
     </row>
-    <row r="740" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="740" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I740" s="2"/>
     </row>
-    <row r="741" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="741" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I741" s="2"/>
     </row>
-    <row r="742" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="742" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I742" s="2"/>
     </row>
-    <row r="743" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="743" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I743" s="2"/>
     </row>
-    <row r="744" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="744" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I744" s="2"/>
     </row>
-    <row r="745" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="745" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I745" s="2"/>
     </row>
-    <row r="746" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="746" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I746" s="2"/>
     </row>
-    <row r="747" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="747" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I747" s="2"/>
     </row>
-    <row r="748" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="748" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I748" s="2"/>
     </row>
-    <row r="749" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="749" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I749" s="2"/>
     </row>
-    <row r="750" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="750" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I750" s="2"/>
     </row>
-    <row r="751" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="751" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I751" s="2"/>
     </row>
-    <row r="752" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="752" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I752" s="2"/>
     </row>
-    <row r="753" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="753" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I753" s="2"/>
     </row>
-    <row r="754" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="754" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I754" s="2"/>
     </row>
-    <row r="755" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="755" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I755" s="2"/>
     </row>
-    <row r="756" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="756" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I756" s="2"/>
     </row>
-    <row r="757" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="757" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I757" s="2"/>
     </row>
-    <row r="758" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="758" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I758" s="2"/>
     </row>
-    <row r="759" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="759" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I759" s="2"/>
     </row>
-    <row r="760" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="760" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I760" s="2"/>
     </row>
-    <row r="761" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="761" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I761" s="2"/>
     </row>
-    <row r="762" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="762" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I762" s="2"/>
     </row>
-    <row r="763" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="763" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I763" s="2"/>
     </row>
-    <row r="764" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="764" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I764" s="2"/>
     </row>
-    <row r="765" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="765" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I765" s="2"/>
     </row>
-    <row r="766" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="766" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I766" s="2"/>
     </row>
-    <row r="767" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="767" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I767" s="2"/>
     </row>
-    <row r="768" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="768" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I768" s="2"/>
     </row>
-    <row r="769" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="769" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I769" s="2"/>
     </row>
-    <row r="770" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="770" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I770" s="2"/>
     </row>
-    <row r="771" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="771" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I771" s="2"/>
     </row>
-    <row r="772" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="772" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I772" s="2"/>
     </row>
-    <row r="773" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="773" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I773" s="2"/>
     </row>
-    <row r="774" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="774" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I774" s="2"/>
     </row>
-    <row r="775" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="775" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I775" s="2"/>
     </row>
-    <row r="776" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="776" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I776" s="2"/>
     </row>
-    <row r="777" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="777" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I777" s="2"/>
     </row>
-    <row r="778" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="778" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I778" s="2"/>
     </row>
-    <row r="779" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="779" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I779" s="2"/>
     </row>
-    <row r="780" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="780" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I780" s="2"/>
     </row>
-    <row r="781" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="781" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I781" s="2"/>
     </row>
-    <row r="782" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="782" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I782" s="2"/>
     </row>
-    <row r="783" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="783" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I783" s="2"/>
     </row>
-    <row r="784" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="784" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I784" s="2"/>
     </row>
-    <row r="785" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="785" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I785" s="2"/>
     </row>
-    <row r="786" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="786" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I786" s="2"/>
     </row>
-    <row r="787" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="787" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I787" s="2"/>
     </row>
-    <row r="788" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="788" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I788" s="2"/>
     </row>
-    <row r="789" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="789" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I789" s="2"/>
     </row>
-    <row r="790" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="790" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I790" s="2"/>
     </row>
-    <row r="791" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="791" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I791" s="2"/>
     </row>
-    <row r="792" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="792" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I792" s="2"/>
     </row>
-    <row r="793" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="793" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I793" s="2"/>
     </row>
-    <row r="794" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="794" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I794" s="2"/>
     </row>
-    <row r="795" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="795" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I795" s="2"/>
     </row>
-    <row r="796" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="796" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I796" s="2"/>
     </row>
-    <row r="797" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="797" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I797" s="2"/>
     </row>
-    <row r="798" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="798" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I798" s="2"/>
     </row>
-    <row r="799" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="799" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I799" s="2"/>
     </row>
-    <row r="800" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="800" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I800" s="2"/>
     </row>
-    <row r="801" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="801" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I801" s="2"/>
     </row>
-    <row r="802" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="802" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I802" s="2"/>
     </row>
-    <row r="803" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="803" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I803" s="2"/>
     </row>
-    <row r="804" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="804" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I804" s="2"/>
     </row>
-    <row r="805" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="805" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I805" s="2"/>
     </row>
-    <row r="806" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="806" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I806" s="2"/>
     </row>
-    <row r="807" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="807" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I807" s="2"/>
     </row>
-    <row r="808" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="808" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I808" s="2"/>
     </row>
-    <row r="809" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="809" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I809" s="2"/>
     </row>
-    <row r="810" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="810" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I810" s="2"/>
     </row>
-    <row r="811" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="811" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I811" s="2"/>
     </row>
-    <row r="812" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="812" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I812" s="2"/>
     </row>
-    <row r="813" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="813" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I813" s="2"/>
     </row>
-    <row r="814" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="814" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I814" s="2"/>
     </row>
-    <row r="815" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="815" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I815" s="2"/>
     </row>
-    <row r="816" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="816" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I816" s="2"/>
     </row>
-    <row r="817" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="817" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I817" s="2"/>
     </row>
-    <row r="818" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="818" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I818" s="2"/>
     </row>
-    <row r="819" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="819" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I819" s="2"/>
     </row>
-    <row r="820" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="820" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I820" s="2"/>
     </row>
-    <row r="821" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="821" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I821" s="2"/>
     </row>
-    <row r="822" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="822" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I822" s="2"/>
     </row>
-    <row r="823" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="823" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I823" s="2"/>
     </row>
-    <row r="824" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="824" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I824" s="2"/>
     </row>
-    <row r="825" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="825" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I825" s="2"/>
     </row>
-    <row r="826" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="826" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I826" s="2"/>
     </row>
-    <row r="827" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="827" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I827" s="2"/>
     </row>
-    <row r="828" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="828" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I828" s="2"/>
     </row>
-    <row r="829" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="829" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I829" s="2"/>
     </row>
-    <row r="830" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="830" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I830" s="2"/>
     </row>
-    <row r="831" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="831" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I831" s="2"/>
     </row>
-    <row r="832" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="832" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I832" s="2"/>
     </row>
-    <row r="833" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="833" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I833" s="2"/>
     </row>
-    <row r="834" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="834" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I834" s="2"/>
     </row>
-    <row r="835" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="835" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I835" s="2"/>
     </row>
-    <row r="836" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="836" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I836" s="2"/>
     </row>
-    <row r="837" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="837" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I837" s="2"/>
     </row>
-    <row r="838" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="838" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I838" s="2"/>
     </row>
-    <row r="839" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="839" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I839" s="2"/>
     </row>
-    <row r="840" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="840" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I840" s="2"/>
     </row>
-    <row r="841" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="841" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I841" s="2"/>
     </row>
-    <row r="842" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="842" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I842" s="2"/>
     </row>
-    <row r="843" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="843" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I843" s="2"/>
     </row>
-    <row r="844" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="844" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I844" s="2"/>
     </row>
-    <row r="845" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="845" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I845" s="2"/>
     </row>
-    <row r="846" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="846" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I846" s="2"/>
     </row>
-    <row r="847" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="847" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I847" s="2"/>
     </row>
-    <row r="848" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="848" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I848" s="2"/>
     </row>
-    <row r="849" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="849" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I849" s="2"/>
     </row>
-    <row r="850" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="850" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I850" s="2"/>
     </row>
-    <row r="851" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="851" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I851" s="2"/>
     </row>
-    <row r="852" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="852" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I852" s="2"/>
     </row>
-    <row r="853" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="853" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I853" s="2"/>
     </row>
-    <row r="854" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="854" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I854" s="2"/>
     </row>
-    <row r="855" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="855" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I855" s="2"/>
     </row>
-    <row r="856" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="856" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I856" s="2"/>
     </row>
-    <row r="857" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="857" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I857" s="2"/>
     </row>
-    <row r="858" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="858" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I858" s="2"/>
     </row>
-    <row r="859" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="859" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I859" s="2"/>
     </row>
-    <row r="860" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="860" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I860" s="2"/>
     </row>
-    <row r="861" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="861" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I861" s="2"/>
     </row>
-    <row r="862" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="862" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I862" s="2"/>
     </row>
-    <row r="863" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="863" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I863" s="2"/>
     </row>
-    <row r="864" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="864" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I864" s="2"/>
     </row>
-    <row r="865" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="865" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I865" s="2"/>
     </row>
-    <row r="866" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="866" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I866" s="2"/>
     </row>
-    <row r="867" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="867" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I867" s="2"/>
     </row>
-    <row r="868" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="868" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I868" s="2"/>
     </row>
-    <row r="869" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="869" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I869" s="2"/>
     </row>
-    <row r="870" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="870" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I870" s="2"/>
     </row>
-    <row r="871" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="871" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I871" s="2"/>
     </row>
-    <row r="872" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="872" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I872" s="2"/>
     </row>
-    <row r="873" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="873" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I873" s="2"/>
     </row>
-    <row r="874" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="874" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I874" s="2"/>
     </row>
-    <row r="875" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="875" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I875" s="2"/>
     </row>
-    <row r="876" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="876" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I876" s="2"/>
     </row>
-    <row r="877" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="877" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I877" s="2"/>
     </row>
-    <row r="878" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="878" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I878" s="2"/>
     </row>
-    <row r="879" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="879" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I879" s="2"/>
     </row>
-    <row r="880" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="880" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I880" s="2"/>
     </row>
-    <row r="881" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="881" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I881" s="2"/>
     </row>
-    <row r="882" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="882" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I882" s="2"/>
     </row>
-    <row r="883" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="883" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I883" s="2"/>
     </row>
-    <row r="884" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="884" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I884" s="2"/>
     </row>
-    <row r="885" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="885" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I885" s="2"/>
     </row>
-    <row r="886" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="886" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I886" s="2"/>
     </row>
-    <row r="887" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="887" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I887" s="2"/>
     </row>
-    <row r="888" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="888" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I888" s="2"/>
     </row>
-    <row r="889" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="889" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I889" s="2"/>
     </row>
-    <row r="890" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="890" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I890" s="2"/>
     </row>
-    <row r="891" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="891" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I891" s="2"/>
     </row>
-    <row r="892" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="892" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I892" s="2"/>
     </row>
-    <row r="893" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="893" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I893" s="2"/>
     </row>
-    <row r="894" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="894" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I894" s="2"/>
     </row>
-    <row r="895" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="895" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I895" s="2"/>
     </row>
-    <row r="896" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="896" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I896" s="2"/>
     </row>
-    <row r="897" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="897" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I897" s="2"/>
     </row>
-    <row r="898" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="898" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I898" s="2"/>
     </row>
-    <row r="899" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="899" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I899" s="2"/>
     </row>
-    <row r="900" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="900" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I900" s="2"/>
     </row>
-    <row r="901" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="901" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I901" s="2"/>
     </row>
-    <row r="902" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="902" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I902" s="2"/>
     </row>
-    <row r="903" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="903" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I903" s="2"/>
     </row>
-    <row r="904" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="904" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I904" s="2"/>
     </row>
-    <row r="905" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="905" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I905" s="2"/>
     </row>
-    <row r="906" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="906" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I906" s="2"/>
     </row>
-    <row r="907" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="907" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I907" s="2"/>
     </row>
-    <row r="908" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="908" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I908" s="2"/>
     </row>
-    <row r="909" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="909" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I909" s="2"/>
     </row>
-    <row r="910" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="910" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I910" s="2"/>
     </row>
-    <row r="911" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="911" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I911" s="2"/>
     </row>
-    <row r="912" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="912" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I912" s="2"/>
     </row>
-    <row r="913" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="913" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I913" s="2"/>
     </row>
-    <row r="914" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="914" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I914" s="2"/>
     </row>
-    <row r="915" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="915" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I915" s="2"/>
     </row>
-    <row r="916" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="916" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I916" s="2"/>
     </row>
-    <row r="917" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="917" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I917" s="2"/>
     </row>
-    <row r="918" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="918" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I918" s="2"/>
     </row>
-    <row r="919" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="919" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I919" s="2"/>
     </row>
-    <row r="920" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="920" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I920" s="2"/>
     </row>
-    <row r="921" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="921" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I921" s="2"/>
     </row>
-    <row r="922" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="922" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I922" s="2"/>
     </row>
-    <row r="923" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="923" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I923" s="2"/>
     </row>
-    <row r="924" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="924" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I924" s="2"/>
     </row>
-    <row r="925" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="925" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I925" s="2"/>
     </row>
-    <row r="926" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="926" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I926" s="2"/>
     </row>
-    <row r="927" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="927" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I927" s="2"/>
     </row>
-    <row r="928" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="928" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I928" s="2"/>
     </row>
-    <row r="929" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="929" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I929" s="2"/>
     </row>
-    <row r="930" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="930" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I930" s="2"/>
     </row>
-    <row r="931" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="931" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I931" s="2"/>
     </row>
-    <row r="932" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="932" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I932" s="2"/>
     </row>
-    <row r="933" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="933" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I933" s="2"/>
     </row>
-    <row r="934" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="934" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I934" s="2"/>
     </row>
-    <row r="935" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="935" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I935" s="2"/>
     </row>
-    <row r="936" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="936" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I936" s="2"/>
     </row>
-    <row r="937" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="937" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I937" s="2"/>
     </row>
-    <row r="938" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="938" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I938" s="2"/>
     </row>
-    <row r="939" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="939" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I939" s="2"/>
     </row>
-    <row r="940" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="940" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I940" s="2"/>
     </row>
-    <row r="941" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="941" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I941" s="2"/>
     </row>
-    <row r="942" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="942" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I942" s="2"/>
     </row>
-    <row r="943" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="943" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I943" s="2"/>
     </row>
-    <row r="944" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="944" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I944" s="2"/>
     </row>
-    <row r="945" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="945" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I945" s="2"/>
     </row>
-    <row r="946" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="946" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I946" s="2"/>
     </row>
-    <row r="947" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="947" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I947" s="2"/>
     </row>
-    <row r="948" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="948" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I948" s="2"/>
     </row>
-    <row r="949" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="949" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I949" s="2"/>
     </row>
-    <row r="950" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="950" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I950" s="2"/>
     </row>
-    <row r="951" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="951" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I951" s="2"/>
     </row>
-    <row r="952" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="952" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I952" s="2"/>
     </row>
-    <row r="953" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="953" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I953" s="2"/>
     </row>
-    <row r="954" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="954" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I954" s="2"/>
     </row>
-    <row r="955" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="955" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I955" s="2"/>
     </row>
-    <row r="956" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="956" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I956" s="2"/>
     </row>
-    <row r="957" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="957" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I957" s="2"/>
     </row>
-    <row r="958" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="958" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I958" s="2"/>
     </row>
-    <row r="959" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="959" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I959" s="2"/>
     </row>
-    <row r="960" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="960" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I960" s="2"/>
     </row>
-    <row r="961" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="961" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I961" s="2"/>
     </row>
-    <row r="962" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="962" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I962" s="2"/>
     </row>
-    <row r="963" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="963" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I963" s="2"/>
     </row>
-    <row r="964" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="964" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I964" s="2"/>
     </row>
-    <row r="965" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="965" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I965" s="2"/>
     </row>
-    <row r="966" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="966" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I966" s="2"/>
     </row>
-    <row r="967" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="967" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I967" s="2"/>
     </row>
-    <row r="968" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="968" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I968" s="2"/>
     </row>
-    <row r="969" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="969" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I969" s="2"/>
     </row>
-    <row r="970" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="970" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I970" s="2"/>
     </row>
-    <row r="971" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="971" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I971" s="2"/>
     </row>
-    <row r="972" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="972" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I972" s="2"/>
     </row>
-    <row r="973" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="973" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I973" s="2"/>
     </row>
-    <row r="974" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="974" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I974" s="2"/>
     </row>
-    <row r="975" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="975" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I975" s="2"/>
     </row>
-    <row r="976" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="976" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I976" s="2"/>
     </row>
-    <row r="977" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="977" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I977" s="2"/>
     </row>
-    <row r="978" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="978" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I978" s="2"/>
     </row>
-    <row r="979" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="979" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I979" s="2"/>
     </row>
-    <row r="980" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="980" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I980" s="2"/>
     </row>
-    <row r="981" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="981" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I981" s="2"/>
     </row>
-    <row r="982" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="982" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I982" s="2"/>
     </row>
-    <row r="983" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="983" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I983" s="2"/>
     </row>
-    <row r="984" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="984" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I984" s="2"/>
     </row>
-    <row r="985" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="985" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I985" s="2"/>
     </row>
-    <row r="986" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="986" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I986" s="2"/>
     </row>
-    <row r="987" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="987" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I987" s="2"/>
     </row>
-    <row r="988" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="988" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I988" s="2"/>
     </row>
-    <row r="989" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="989" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I989" s="2"/>
     </row>
-    <row r="990" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="990" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I990" s="2"/>
     </row>
-    <row r="991" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="991" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I991" s="2"/>
     </row>
-    <row r="992" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="992" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I992" s="2"/>
     </row>
-    <row r="993" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="993" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I993" s="2"/>
     </row>
-    <row r="994" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="994" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I994" s="2"/>
     </row>
-    <row r="995" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="995" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I995" s="2"/>
     </row>
-    <row r="996" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="996" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I996" s="2"/>
     </row>
-    <row r="997" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="997" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I997" s="2"/>
     </row>
-    <row r="998" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="998" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I998" s="2"/>
     </row>
-    <row r="999" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="999" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I999" s="2"/>
     </row>
-    <row r="1000" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1000" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1000" s="2"/>
     </row>
-    <row r="1001" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1001" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1001" s="2"/>
     </row>
-    <row r="1002" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1002" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1002" s="2"/>
     </row>
-    <row r="1003" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1003" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1003" s="2"/>
     </row>
-    <row r="1004" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1004" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1004" s="2"/>
     </row>
-    <row r="1005" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1005" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1005" s="2"/>
     </row>
-    <row r="1006" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1006" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1006" s="2"/>
     </row>
-    <row r="1007" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1007" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1007" s="2"/>
     </row>
-    <row r="1008" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1008" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1008" s="2"/>
     </row>
-    <row r="1009" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1009" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1009" s="2"/>
     </row>
-    <row r="1010" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1010" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1010" s="2"/>
     </row>
-    <row r="1011" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1011" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1011" s="2"/>
     </row>
-    <row r="1012" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1012" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1012" s="2"/>
     </row>
-    <row r="1013" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1013" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1013" s="2"/>
     </row>
-    <row r="1014" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1014" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1014" s="2"/>
     </row>
-    <row r="1015" spans="9:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1015" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I1015" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish i type instructions, just LW and SW left for week 2 deliverables
</commit_message>
<xml_diff>
--- a/Final-Project/instruction_set.xlsx
+++ b/Final-Project/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhodson/GitHub/digital-design/Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24214E34-06DB-384C-AE68-029E0FE03F8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C6A40-F4C2-EC4A-8001-D8AED24B7A1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="172">
   <si>
     <t>Category</t>
   </si>
@@ -526,13 +526,16 @@
     <t>Multiplies (unsigned) $s by $t and stores the lower half of the result in $LO and the upper half in $HI.</t>
   </si>
   <si>
-    <t>31 downto 26</t>
-  </si>
-  <si>
-    <t>5 downto 0</t>
-  </si>
-  <si>
     <t>r type</t>
+  </si>
+  <si>
+    <t>i type</t>
+  </si>
+  <si>
+    <t>IR(31 downto 26)</t>
+  </si>
+  <si>
+    <t>IR(5 downto 0)</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +582,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -592,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -602,9 +617,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -619,6 +631,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -975,10 +996,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -1016,517 +1037,531 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="9"/>
+      <c r="I3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="L3" s="13" t="s">
-        <v>170</v>
+      <c r="J3" s="12"/>
+      <c r="L3" s="12" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="17" t="s">
         <v>21</v>
       </c>
+      <c r="J4" s="14"/>
+      <c r="L4" s="14" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="12" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="12" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="13"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="12" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="13"/>
+      <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="12" t="s">
+      <c r="H15" s="9"/>
+      <c r="I15" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="J15" s="13"/>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="12" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="J16" s="13"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="12" t="s">
+      <c r="H17" s="9"/>
+      <c r="I17" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="J17" s="13"/>
+      <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="12" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="13"/>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="13"/>
+      <c r="I19" s="17" t="s">
         <v>89</v>
       </c>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10" ht="99" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="13"/>
+      <c r="I20" s="17" t="s">
         <v>93</v>
       </c>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="12" t="s">
+      <c r="H21" s="9"/>
+      <c r="I21" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="J21" s="13"/>
+      <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="12" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J22" s="13"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="12" t="s">
+      <c r="H23" s="9"/>
+      <c r="I23" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="13"/>
+      <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
@@ -1537,7 +1572,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="6"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1560,7 +1595,7 @@
         <v>10</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="5" t="s">
         <v>113</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -1584,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="5" t="s">
         <v>117</v>
       </c>
       <c r="J26" s="1" t="s">
@@ -1592,7 +1627,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I27" s="6"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -1615,7 +1650,7 @@
         <v>10</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="5" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1629,14 +1664,14 @@
       <c r="E29" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="8" t="s">
         <v>160</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1657,7 +1692,7 @@
         <v>10</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="5" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1678,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="5" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1699,16 +1734,16 @@
         <v>10</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="7"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="4" t="s">
         <v>139</v>
       </c>
@@ -1722,13 +1757,13 @@
         <v>10</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D34" s="8"/>
-      <c r="I34" s="6"/>
+      <c r="D34" s="7"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -1736,8 +1771,8 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="8"/>
-      <c r="I35" s="6"/>
+      <c r="D35" s="7"/>
+      <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
@@ -1756,7 +1791,7 @@
         <v>10</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="5" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1777,412 +1812,412 @@
         <v>10</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="12" t="s">
+      <c r="H38" s="9"/>
+      <c r="I38" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="J38" s="13"/>
+      <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I39" s="6"/>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I40" s="6"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I41" s="6"/>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I42" s="6"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I43" s="6"/>
+      <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I44" s="6"/>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I45" s="6"/>
+      <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I46" s="6"/>
+      <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I47" s="6"/>
+      <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I48" s="6"/>
+      <c r="I48" s="5"/>
     </row>
     <row r="49" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I49" s="6"/>
+      <c r="I49" s="5"/>
     </row>
     <row r="50" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I50" s="6"/>
+      <c r="I50" s="5"/>
     </row>
     <row r="51" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I51" s="6"/>
+      <c r="I51" s="5"/>
     </row>
     <row r="52" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I52" s="6"/>
+      <c r="I52" s="5"/>
     </row>
     <row r="53" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I53" s="6"/>
+      <c r="I53" s="5"/>
     </row>
     <row r="54" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I54" s="6"/>
+      <c r="I54" s="5"/>
     </row>
     <row r="55" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I55" s="6"/>
+      <c r="I55" s="5"/>
     </row>
     <row r="56" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I56" s="6"/>
+      <c r="I56" s="5"/>
     </row>
     <row r="57" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I57" s="6"/>
+      <c r="I57" s="5"/>
     </row>
     <row r="58" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I58" s="6"/>
+      <c r="I58" s="5"/>
     </row>
     <row r="59" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I59" s="6"/>
+      <c r="I59" s="5"/>
     </row>
     <row r="60" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I60" s="6"/>
+      <c r="I60" s="5"/>
     </row>
     <row r="61" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I61" s="6"/>
+      <c r="I61" s="5"/>
     </row>
     <row r="62" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I62" s="6"/>
+      <c r="I62" s="5"/>
     </row>
     <row r="63" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I63" s="6"/>
+      <c r="I63" s="5"/>
     </row>
     <row r="64" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I64" s="6"/>
+      <c r="I64" s="5"/>
     </row>
     <row r="65" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I65" s="6"/>
+      <c r="I65" s="5"/>
     </row>
     <row r="66" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I66" s="6"/>
+      <c r="I66" s="5"/>
     </row>
     <row r="67" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I67" s="6"/>
+      <c r="I67" s="5"/>
     </row>
     <row r="68" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I68" s="6"/>
+      <c r="I68" s="5"/>
     </row>
     <row r="69" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I69" s="6"/>
+      <c r="I69" s="5"/>
     </row>
     <row r="70" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I70" s="6"/>
+      <c r="I70" s="5"/>
     </row>
     <row r="71" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I71" s="6"/>
+      <c r="I71" s="5"/>
     </row>
     <row r="72" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I72" s="6"/>
+      <c r="I72" s="5"/>
     </row>
     <row r="73" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I73" s="6"/>
+      <c r="I73" s="5"/>
     </row>
     <row r="74" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I74" s="6"/>
+      <c r="I74" s="5"/>
     </row>
     <row r="75" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I75" s="6"/>
+      <c r="I75" s="5"/>
     </row>
     <row r="76" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I76" s="6"/>
+      <c r="I76" s="5"/>
     </row>
     <row r="77" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I77" s="6"/>
+      <c r="I77" s="5"/>
     </row>
     <row r="78" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I78" s="6"/>
+      <c r="I78" s="5"/>
     </row>
     <row r="79" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I79" s="6"/>
+      <c r="I79" s="5"/>
     </row>
     <row r="80" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I80" s="6"/>
+      <c r="I80" s="5"/>
     </row>
     <row r="81" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I81" s="6"/>
+      <c r="I81" s="5"/>
     </row>
     <row r="82" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I82" s="6"/>
+      <c r="I82" s="5"/>
     </row>
     <row r="83" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I83" s="6"/>
+      <c r="I83" s="5"/>
     </row>
     <row r="84" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I84" s="6"/>
+      <c r="I84" s="5"/>
     </row>
     <row r="85" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I85" s="6"/>
+      <c r="I85" s="5"/>
     </row>
     <row r="86" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I86" s="6"/>
+      <c r="I86" s="5"/>
     </row>
     <row r="87" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I87" s="6"/>
+      <c r="I87" s="5"/>
     </row>
     <row r="88" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I88" s="6"/>
+      <c r="I88" s="5"/>
     </row>
     <row r="89" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I89" s="6"/>
+      <c r="I89" s="5"/>
     </row>
     <row r="90" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I90" s="6"/>
+      <c r="I90" s="5"/>
     </row>
     <row r="91" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I91" s="6"/>
+      <c r="I91" s="5"/>
     </row>
     <row r="92" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I92" s="6"/>
+      <c r="I92" s="5"/>
     </row>
     <row r="93" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I93" s="6"/>
+      <c r="I93" s="5"/>
     </row>
     <row r="94" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I94" s="6"/>
+      <c r="I94" s="5"/>
     </row>
     <row r="95" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I95" s="6"/>
+      <c r="I95" s="5"/>
     </row>
     <row r="96" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I96" s="6"/>
+      <c r="I96" s="5"/>
     </row>
     <row r="97" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I97" s="6"/>
+      <c r="I97" s="5"/>
     </row>
     <row r="98" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I98" s="6"/>
+      <c r="I98" s="5"/>
     </row>
     <row r="99" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I99" s="6"/>
+      <c r="I99" s="5"/>
     </row>
     <row r="100" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I100" s="6"/>
+      <c r="I100" s="5"/>
     </row>
     <row r="101" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I101" s="6"/>
+      <c r="I101" s="5"/>
     </row>
     <row r="102" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I102" s="6"/>
+      <c r="I102" s="5"/>
     </row>
     <row r="103" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I103" s="6"/>
+      <c r="I103" s="5"/>
     </row>
     <row r="104" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I104" s="6"/>
+      <c r="I104" s="5"/>
     </row>
     <row r="105" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I105" s="6"/>
+      <c r="I105" s="5"/>
     </row>
     <row r="106" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I106" s="6"/>
+      <c r="I106" s="5"/>
     </row>
     <row r="107" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I107" s="6"/>
+      <c r="I107" s="5"/>
     </row>
     <row r="108" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I108" s="6"/>
+      <c r="I108" s="5"/>
     </row>
     <row r="109" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I109" s="6"/>
+      <c r="I109" s="5"/>
     </row>
     <row r="110" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I110" s="6"/>
+      <c r="I110" s="5"/>
     </row>
     <row r="111" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I111" s="6"/>
+      <c r="I111" s="5"/>
     </row>
     <row r="112" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I112" s="6"/>
+      <c r="I112" s="5"/>
     </row>
     <row r="113" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I113" s="6"/>
+      <c r="I113" s="5"/>
     </row>
     <row r="114" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I114" s="6"/>
+      <c r="I114" s="5"/>
     </row>
     <row r="115" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I115" s="6"/>
+      <c r="I115" s="5"/>
     </row>
     <row r="116" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I116" s="6"/>
+      <c r="I116" s="5"/>
     </row>
     <row r="117" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I117" s="6"/>
+      <c r="I117" s="5"/>
     </row>
     <row r="118" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I118" s="6"/>
+      <c r="I118" s="5"/>
     </row>
     <row r="119" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I119" s="6"/>
+      <c r="I119" s="5"/>
     </row>
     <row r="120" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I120" s="6"/>
+      <c r="I120" s="5"/>
     </row>
     <row r="121" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I121" s="6"/>
+      <c r="I121" s="5"/>
     </row>
     <row r="122" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I122" s="6"/>
+      <c r="I122" s="5"/>
     </row>
     <row r="123" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I123" s="6"/>
+      <c r="I123" s="5"/>
     </row>
     <row r="124" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I124" s="6"/>
+      <c r="I124" s="5"/>
     </row>
     <row r="125" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I125" s="6"/>
+      <c r="I125" s="5"/>
     </row>
     <row r="126" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I126" s="6"/>
+      <c r="I126" s="5"/>
     </row>
     <row r="127" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I127" s="6"/>
+      <c r="I127" s="5"/>
     </row>
     <row r="128" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I128" s="6"/>
+      <c r="I128" s="5"/>
     </row>
     <row r="129" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I129" s="6"/>
+      <c r="I129" s="5"/>
     </row>
     <row r="130" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I130" s="6"/>
+      <c r="I130" s="5"/>
     </row>
     <row r="131" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I131" s="6"/>
+      <c r="I131" s="5"/>
     </row>
     <row r="132" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I132" s="6"/>
+      <c r="I132" s="5"/>
     </row>
     <row r="133" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I133" s="6"/>
+      <c r="I133" s="5"/>
     </row>
     <row r="134" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I134" s="6"/>
+      <c r="I134" s="5"/>
     </row>
     <row r="135" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I135" s="6"/>
+      <c r="I135" s="5"/>
     </row>
     <row r="136" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I136" s="6"/>
+      <c r="I136" s="5"/>
     </row>
     <row r="137" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I137" s="6"/>
+      <c r="I137" s="5"/>
     </row>
     <row r="138" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I138" s="6"/>
+      <c r="I138" s="5"/>
     </row>
     <row r="139" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I139" s="6"/>
+      <c r="I139" s="5"/>
     </row>
     <row r="140" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I140" s="6"/>
+      <c r="I140" s="5"/>
     </row>
     <row r="141" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I141" s="6"/>
+      <c r="I141" s="5"/>
     </row>
     <row r="142" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I142" s="6"/>
+      <c r="I142" s="5"/>
     </row>
     <row r="143" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I143" s="6"/>
+      <c r="I143" s="5"/>
     </row>
     <row r="144" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I144" s="6"/>
+      <c r="I144" s="5"/>
     </row>
     <row r="145" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I145" s="6"/>
+      <c r="I145" s="5"/>
     </row>
     <row r="146" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I146" s="6"/>
+      <c r="I146" s="5"/>
     </row>
     <row r="147" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I147" s="6"/>
+      <c r="I147" s="5"/>
     </row>
     <row r="148" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I148" s="6"/>
+      <c r="I148" s="5"/>
     </row>
     <row r="149" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I149" s="6"/>
+      <c r="I149" s="5"/>
     </row>
     <row r="150" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I150" s="6"/>
+      <c r="I150" s="5"/>
     </row>
     <row r="151" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I151" s="6"/>
+      <c r="I151" s="5"/>
     </row>
     <row r="152" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I152" s="6"/>
+      <c r="I152" s="5"/>
     </row>
     <row r="153" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I153" s="6"/>
+      <c r="I153" s="5"/>
     </row>
     <row r="154" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I154" s="6"/>
+      <c r="I154" s="5"/>
     </row>
     <row r="155" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I155" s="6"/>
+      <c r="I155" s="5"/>
     </row>
     <row r="156" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I156" s="6"/>
+      <c r="I156" s="5"/>
     </row>
     <row r="157" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I157" s="6"/>
+      <c r="I157" s="5"/>
     </row>
     <row r="158" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I158" s="6"/>
+      <c r="I158" s="5"/>
     </row>
     <row r="159" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I159" s="6"/>
+      <c r="I159" s="5"/>
     </row>
     <row r="160" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I160" s="6"/>
+      <c r="I160" s="5"/>
     </row>
     <row r="161" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I161" s="6"/>
+      <c r="I161" s="5"/>
     </row>
     <row r="162" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I162" s="6"/>
+      <c r="I162" s="5"/>
     </row>
     <row r="163" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I163" s="6"/>
+      <c r="I163" s="5"/>
     </row>
     <row r="164" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I164" s="6"/>
+      <c r="I164" s="5"/>
     </row>
     <row r="165" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I165" s="2"/>

</xml_diff>

<commit_message>
branch instructions working ?
</commit_message>
<xml_diff>
--- a/Final-Project/instruction_set.xlsx
+++ b/Final-Project/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhodson/GitHub/digital-design/Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C6A40-F4C2-EC4A-8001-D8AED24B7A1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F984C0F-F0A5-5347-AA2E-3215ABA70285}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="174">
   <si>
     <t>Category</t>
   </si>
@@ -490,12 +490,6 @@
     <t>These arithmetic shifts, if signed bit is 1, will append 1s. If signed bit is 0, will append 0s.  H is an 5-bit immediate value stored in bits 10-6 of the instruction register.</t>
   </si>
   <si>
-    <t>IsSigned = false</t>
-  </si>
-  <si>
-    <t>yes (will be changed in future classes)</t>
-  </si>
-  <si>
     <t>0x0A</t>
   </si>
   <si>
@@ -536,6 +530,18 @@
   </si>
   <si>
     <t>IR(5 downto 0)</t>
+  </si>
+  <si>
+    <t>isSigned</t>
+  </si>
+  <si>
+    <t>load word store word</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>jump</t>
   </si>
 </sst>
 </file>
@@ -563,18 +569,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -594,6 +594,30 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -607,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -616,28 +640,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="229" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -992,14 +1035,15 @@
     <col min="6" max="6" width="38" customWidth="1"/>
     <col min="7" max="8" width="6.6640625" customWidth="1"/>
     <col min="9" max="9" width="75.5" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -1030,538 +1074,556 @@
         <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>156</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="11" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="L3" s="12" t="s">
-        <v>168</v>
+      <c r="J3" s="10"/>
+      <c r="L3" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="L4" s="14" t="s">
-        <v>169</v>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="11" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="10"/>
+      <c r="L5" s="19" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="17" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="J7" s="12"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="L7" s="30" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="J8" s="12"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="11" t="s">
+      <c r="H9" s="7"/>
+      <c r="I9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="12"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="17" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="C13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="13" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="13" t="s">
+      <c r="H14" s="11"/>
+      <c r="I14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
+      <c r="H15" s="7"/>
+      <c r="I15" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="C16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="13" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="J14" s="13" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
+      <c r="H18" s="7"/>
+      <c r="I18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B19" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="99" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="C21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
+      <c r="H21" s="7"/>
+      <c r="I21" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="1:10" ht="43" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="9" t="s">
+      <c r="C23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B17" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B19" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" ht="99" x14ac:dyDescent="0.2">
-      <c r="B20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B22" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B23" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="11" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="12"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
@@ -1572,198 +1634,216 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="5"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="5" t="s">
+      <c r="H25" s="16"/>
+      <c r="I25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>157</v>
+      <c r="J25" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="43" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="5" t="s">
+      <c r="H26" s="16"/>
+      <c r="I26" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>157</v>
+      <c r="J26" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I27" s="5"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="20"/>
+      <c r="I28" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="B29" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="23"/>
+      <c r="D29" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="20"/>
+      <c r="I29" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" s="23"/>
+    </row>
+    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="B30" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G30" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="8" t="s">
+      <c r="H30" s="20"/>
+      <c r="I30" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" s="23"/>
+    </row>
+    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G31" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="H31" s="20"/>
+      <c r="I31" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="B32" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G32" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="H32" s="20"/>
+      <c r="I32" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="J32" s="23"/>
+    </row>
+    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G33" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-      <c r="B33" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="5" t="s">
+      <c r="H33" s="20"/>
+      <c r="I33" s="22" t="s">
         <v>141</v>
       </c>
+      <c r="J33" s="23"/>
     </row>
     <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D34" s="7"/>
-      <c r="I34" s="5"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -1771,453 +1851,457 @@
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="7"/>
-      <c r="I35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="28"/>
+      <c r="D36" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="5" t="s">
+      <c r="H36" s="27"/>
+      <c r="I36" s="30" t="s">
         <v>146</v>
       </c>
+      <c r="J36" s="28"/>
     </row>
     <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="28"/>
+      <c r="D37" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="F37" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="5" t="s">
+      <c r="H37" s="27"/>
+      <c r="I37" s="30" t="s">
         <v>149</v>
       </c>
+      <c r="J37" s="28"/>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.2">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="9"/>
-      <c r="I38" s="11" t="s">
+      <c r="H38" s="7"/>
+      <c r="I38" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="J38" s="12"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I39" s="5"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I40" s="5"/>
+      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I41" s="5"/>
+      <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I42" s="5"/>
+      <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I43" s="5"/>
+      <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I44" s="5"/>
+      <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I45" s="5"/>
+      <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I46" s="5"/>
+      <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I47" s="5"/>
+      <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:10" ht="13" x14ac:dyDescent="0.15">
-      <c r="I48" s="5"/>
+      <c r="I48" s="4"/>
     </row>
     <row r="49" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I49" s="5"/>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I50" s="5"/>
+      <c r="I50" s="4"/>
     </row>
     <row r="51" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I51" s="5"/>
+      <c r="I51" s="4"/>
     </row>
     <row r="52" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I52" s="5"/>
+      <c r="I52" s="4"/>
     </row>
     <row r="53" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I53" s="5"/>
+      <c r="I53" s="4"/>
     </row>
     <row r="54" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I54" s="5"/>
+      <c r="I54" s="4"/>
     </row>
     <row r="55" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I55" s="5"/>
+      <c r="I55" s="4"/>
     </row>
     <row r="56" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I56" s="5"/>
+      <c r="I56" s="4"/>
     </row>
     <row r="57" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I57" s="5"/>
+      <c r="I57" s="4"/>
     </row>
     <row r="58" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I58" s="5"/>
+      <c r="I58" s="4"/>
     </row>
     <row r="59" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I59" s="5"/>
+      <c r="I59" s="4"/>
     </row>
     <row r="60" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I60" s="5"/>
+      <c r="I60" s="4"/>
     </row>
     <row r="61" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I61" s="5"/>
+      <c r="I61" s="4"/>
     </row>
     <row r="62" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I62" s="5"/>
+      <c r="I62" s="4"/>
     </row>
     <row r="63" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I63" s="5"/>
+      <c r="I63" s="4"/>
     </row>
     <row r="64" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I64" s="5"/>
+      <c r="I64" s="4"/>
     </row>
     <row r="65" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I65" s="5"/>
+      <c r="I65" s="4"/>
     </row>
     <row r="66" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I66" s="5"/>
+      <c r="I66" s="4"/>
     </row>
     <row r="67" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I67" s="5"/>
+      <c r="I67" s="4"/>
     </row>
     <row r="68" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I68" s="5"/>
+      <c r="I68" s="4"/>
     </row>
     <row r="69" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I69" s="5"/>
+      <c r="I69" s="4"/>
     </row>
     <row r="70" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I70" s="5"/>
+      <c r="I70" s="4"/>
     </row>
     <row r="71" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I71" s="5"/>
+      <c r="I71" s="4"/>
     </row>
     <row r="72" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I72" s="5"/>
+      <c r="I72" s="4"/>
     </row>
     <row r="73" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I73" s="5"/>
+      <c r="I73" s="4"/>
     </row>
     <row r="74" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I74" s="5"/>
+      <c r="I74" s="4"/>
     </row>
     <row r="75" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I75" s="5"/>
+      <c r="I75" s="4"/>
     </row>
     <row r="76" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I76" s="5"/>
+      <c r="I76" s="4"/>
     </row>
     <row r="77" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I77" s="5"/>
+      <c r="I77" s="4"/>
     </row>
     <row r="78" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I78" s="5"/>
+      <c r="I78" s="4"/>
     </row>
     <row r="79" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I79" s="5"/>
+      <c r="I79" s="4"/>
     </row>
     <row r="80" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I80" s="5"/>
+      <c r="I80" s="4"/>
     </row>
     <row r="81" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I81" s="5"/>
+      <c r="I81" s="4"/>
     </row>
     <row r="82" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I82" s="5"/>
+      <c r="I82" s="4"/>
     </row>
     <row r="83" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I83" s="5"/>
+      <c r="I83" s="4"/>
     </row>
     <row r="84" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I84" s="5"/>
+      <c r="I84" s="4"/>
     </row>
     <row r="85" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I85" s="5"/>
+      <c r="I85" s="4"/>
     </row>
     <row r="86" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I86" s="5"/>
+      <c r="I86" s="4"/>
     </row>
     <row r="87" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I87" s="5"/>
+      <c r="I87" s="4"/>
     </row>
     <row r="88" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I88" s="5"/>
+      <c r="I88" s="4"/>
     </row>
     <row r="89" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I89" s="5"/>
+      <c r="I89" s="4"/>
     </row>
     <row r="90" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I90" s="5"/>
+      <c r="I90" s="4"/>
     </row>
     <row r="91" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I91" s="5"/>
+      <c r="I91" s="4"/>
     </row>
     <row r="92" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I92" s="5"/>
+      <c r="I92" s="4"/>
     </row>
     <row r="93" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I93" s="5"/>
+      <c r="I93" s="4"/>
     </row>
     <row r="94" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I94" s="5"/>
+      <c r="I94" s="4"/>
     </row>
     <row r="95" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I95" s="5"/>
+      <c r="I95" s="4"/>
     </row>
     <row r="96" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I96" s="5"/>
+      <c r="I96" s="4"/>
     </row>
     <row r="97" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I97" s="5"/>
+      <c r="I97" s="4"/>
     </row>
     <row r="98" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I98" s="5"/>
+      <c r="I98" s="4"/>
     </row>
     <row r="99" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I99" s="5"/>
+      <c r="I99" s="4"/>
     </row>
     <row r="100" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I100" s="5"/>
+      <c r="I100" s="4"/>
     </row>
     <row r="101" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I101" s="5"/>
+      <c r="I101" s="4"/>
     </row>
     <row r="102" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I102" s="5"/>
+      <c r="I102" s="4"/>
     </row>
     <row r="103" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I103" s="5"/>
+      <c r="I103" s="4"/>
     </row>
     <row r="104" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I104" s="5"/>
+      <c r="I104" s="4"/>
     </row>
     <row r="105" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I105" s="5"/>
+      <c r="I105" s="4"/>
     </row>
     <row r="106" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I106" s="5"/>
+      <c r="I106" s="4"/>
     </row>
     <row r="107" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I107" s="5"/>
+      <c r="I107" s="4"/>
     </row>
     <row r="108" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I108" s="5"/>
+      <c r="I108" s="4"/>
     </row>
     <row r="109" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I109" s="5"/>
+      <c r="I109" s="4"/>
     </row>
     <row r="110" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I110" s="5"/>
+      <c r="I110" s="4"/>
     </row>
     <row r="111" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I111" s="5"/>
+      <c r="I111" s="4"/>
     </row>
     <row r="112" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I112" s="5"/>
+      <c r="I112" s="4"/>
     </row>
     <row r="113" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I113" s="5"/>
+      <c r="I113" s="4"/>
     </row>
     <row r="114" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I114" s="5"/>
+      <c r="I114" s="4"/>
     </row>
     <row r="115" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I115" s="5"/>
+      <c r="I115" s="4"/>
     </row>
     <row r="116" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I116" s="5"/>
+      <c r="I116" s="4"/>
     </row>
     <row r="117" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I117" s="5"/>
+      <c r="I117" s="4"/>
     </row>
     <row r="118" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I118" s="5"/>
+      <c r="I118" s="4"/>
     </row>
     <row r="119" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I119" s="5"/>
+      <c r="I119" s="4"/>
     </row>
     <row r="120" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I120" s="5"/>
+      <c r="I120" s="4"/>
     </row>
     <row r="121" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I121" s="5"/>
+      <c r="I121" s="4"/>
     </row>
     <row r="122" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I122" s="5"/>
+      <c r="I122" s="4"/>
     </row>
     <row r="123" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I123" s="5"/>
+      <c r="I123" s="4"/>
     </row>
     <row r="124" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I124" s="5"/>
+      <c r="I124" s="4"/>
     </row>
     <row r="125" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I125" s="5"/>
+      <c r="I125" s="4"/>
     </row>
     <row r="126" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I126" s="5"/>
+      <c r="I126" s="4"/>
     </row>
     <row r="127" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I127" s="5"/>
+      <c r="I127" s="4"/>
     </row>
     <row r="128" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I128" s="5"/>
+      <c r="I128" s="4"/>
     </row>
     <row r="129" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I129" s="5"/>
+      <c r="I129" s="4"/>
     </row>
     <row r="130" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I130" s="5"/>
+      <c r="I130" s="4"/>
     </row>
     <row r="131" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I131" s="5"/>
+      <c r="I131" s="4"/>
     </row>
     <row r="132" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I132" s="5"/>
+      <c r="I132" s="4"/>
     </row>
     <row r="133" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I133" s="5"/>
+      <c r="I133" s="4"/>
     </row>
     <row r="134" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I134" s="5"/>
+      <c r="I134" s="4"/>
     </row>
     <row r="135" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I135" s="5"/>
+      <c r="I135" s="4"/>
     </row>
     <row r="136" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I136" s="5"/>
+      <c r="I136" s="4"/>
     </row>
     <row r="137" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I137" s="5"/>
+      <c r="I137" s="4"/>
     </row>
     <row r="138" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I138" s="5"/>
+      <c r="I138" s="4"/>
     </row>
     <row r="139" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I139" s="5"/>
+      <c r="I139" s="4"/>
     </row>
     <row r="140" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I140" s="5"/>
+      <c r="I140" s="4"/>
     </row>
     <row r="141" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I141" s="5"/>
+      <c r="I141" s="4"/>
     </row>
     <row r="142" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I142" s="5"/>
+      <c r="I142" s="4"/>
     </row>
     <row r="143" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I143" s="5"/>
+      <c r="I143" s="4"/>
     </row>
     <row r="144" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I144" s="5"/>
+      <c r="I144" s="4"/>
     </row>
     <row r="145" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I145" s="5"/>
+      <c r="I145" s="4"/>
     </row>
     <row r="146" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I146" s="5"/>
+      <c r="I146" s="4"/>
     </row>
     <row r="147" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I147" s="5"/>
+      <c r="I147" s="4"/>
     </row>
     <row r="148" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I148" s="5"/>
+      <c r="I148" s="4"/>
     </row>
     <row r="149" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I149" s="5"/>
+      <c r="I149" s="4"/>
     </row>
     <row r="150" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I150" s="5"/>
+      <c r="I150" s="4"/>
     </row>
     <row r="151" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I151" s="5"/>
+      <c r="I151" s="4"/>
     </row>
     <row r="152" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I152" s="5"/>
+      <c r="I152" s="4"/>
     </row>
     <row r="153" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I153" s="5"/>
+      <c r="I153" s="4"/>
     </row>
     <row r="154" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I154" s="5"/>
+      <c r="I154" s="4"/>
     </row>
     <row r="155" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I155" s="5"/>
+      <c r="I155" s="4"/>
     </row>
     <row r="156" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I156" s="5"/>
+      <c r="I156" s="4"/>
     </row>
     <row r="157" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I157" s="5"/>
+      <c r="I157" s="4"/>
     </row>
     <row r="158" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I158" s="5"/>
+      <c r="I158" s="4"/>
     </row>
     <row r="159" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I159" s="5"/>
+      <c r="I159" s="4"/>
     </row>
     <row r="160" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I160" s="5"/>
+      <c r="I160" s="4"/>
     </row>
     <row r="161" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I161" s="5"/>
+      <c r="I161" s="4"/>
     </row>
     <row r="162" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I162" s="5"/>
+      <c r="I162" s="4"/>
     </row>
     <row r="163" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I163" s="5"/>
+      <c r="I163" s="4"/>
     </row>
     <row r="164" spans="9:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="I164" s="5"/>
+      <c r="I164" s="4"/>
     </row>
     <row r="165" spans="9:9" ht="13" x14ac:dyDescent="0.15">
       <c r="I165" s="2"/>

</xml_diff>

<commit_message>
finsih project? testing required
</commit_message>
<xml_diff>
--- a/Final-Project/instruction_set.xlsx
+++ b/Final-Project/instruction_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnhodson/GitHub/digital-design/Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F984C0F-F0A5-5347-AA2E-3215ABA70285}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3616B15C-8401-0849-8FDB-E471D0E756B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -676,11 +676,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1023,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" zoomScaleNormal="229" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" zoomScaleNormal="229" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1217,7 +1221,7 @@
         <v>164</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="29" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1835,15 +1839,15 @@
       <c r="J33" s="23"/>
     </row>
     <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="23"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -1855,50 +1859,50 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29" t="s">
+      <c r="C36" s="27"/>
+      <c r="D36" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F36" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="G36" s="27" t="s">
+      <c r="G36" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="27"/>
-      <c r="I36" s="30" t="s">
+      <c r="H36" s="26"/>
+      <c r="I36" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="J36" s="28"/>
+      <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29" t="s">
+      <c r="C37" s="27"/>
+      <c r="D37" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="27"/>
-      <c r="I37" s="30" t="s">
+      <c r="H37" s="26"/>
+      <c r="I37" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="J37" s="28"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">

</xml_diff>